<commit_message>
update 20231102 by xhx
</commit_message>
<xml_diff>
--- a/rules/start-end effect/rules_SE.xlsx
+++ b/rules/start-end effect/rules_SE.xlsx
@@ -1428,7 +1428,7 @@
         <v>23</v>
       </c>
       <c r="K27" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L27" s="0"/>
       <c r="M27" s="0"/>
@@ -1469,7 +1469,7 @@
         <v>23</v>
       </c>
       <c r="K28" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L28" s="0">
         <v>0.029999999999999999</v>
@@ -1516,7 +1516,7 @@
         <v>23</v>
       </c>
       <c r="K29" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L29" s="0">
         <v>0.029999999999999999</v>
@@ -1563,7 +1563,7 @@
         <v>23</v>
       </c>
       <c r="K30" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L30" s="0">
         <v>0.029999999999999999</v>
@@ -1610,7 +1610,7 @@
         <v>23</v>
       </c>
       <c r="K31" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L31" s="0">
         <v>0.040000000000000001</v>
@@ -1657,7 +1657,7 @@
         <v>23</v>
       </c>
       <c r="K32" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L32" s="0">
         <v>0.040000000000000001</v>
@@ -1704,7 +1704,7 @@
         <v>23</v>
       </c>
       <c r="K33" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L33" s="0">
         <v>0.040000000000000001</v>
@@ -1751,7 +1751,7 @@
         <v>23</v>
       </c>
       <c r="K34" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L34" s="0">
         <v>0.050000000000000003</v>
@@ -1798,7 +1798,7 @@
         <v>23</v>
       </c>
       <c r="K35" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L35" s="0">
         <v>0.050000000000000003</v>
@@ -1845,7 +1845,7 @@
         <v>23</v>
       </c>
       <c r="K36" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L36" s="0">
         <v>0.050000000000000003</v>
@@ -1892,7 +1892,7 @@
         <v>23</v>
       </c>
       <c r="K37" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L37" s="0">
         <v>0.059999999999999998</v>
@@ -1939,7 +1939,7 @@
         <v>23</v>
       </c>
       <c r="K38" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L38" s="0">
         <v>0.059999999999999998</v>
@@ -1986,7 +1986,7 @@
         <v>23</v>
       </c>
       <c r="K39" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L39" s="0">
         <v>0.059999999999999998</v>
@@ -2033,7 +2033,7 @@
         <v>23</v>
       </c>
       <c r="K40" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L40" s="0">
         <v>0.070000000000000007</v>
@@ -2080,7 +2080,7 @@
         <v>23</v>
       </c>
       <c r="K41" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L41" s="0">
         <v>0.070000000000000007</v>
@@ -2127,7 +2127,7 @@
         <v>23</v>
       </c>
       <c r="K42" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L42" s="0">
         <v>0.070000000000000007</v>
@@ -2174,7 +2174,7 @@
         <v>23</v>
       </c>
       <c r="K43" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L43" s="0">
         <v>0.080000000000000002</v>
@@ -2221,7 +2221,7 @@
         <v>23</v>
       </c>
       <c r="K44" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L44" s="0">
         <v>0.080000000000000002</v>
@@ -2268,7 +2268,7 @@
         <v>23</v>
       </c>
       <c r="K45" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L45" s="0">
         <v>0.080000000000000002</v>
@@ -2315,7 +2315,7 @@
         <v>23</v>
       </c>
       <c r="K46" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L46" s="0">
         <v>0.089999999999999997</v>
@@ -2362,7 +2362,7 @@
         <v>23</v>
       </c>
       <c r="K47" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L47" s="0">
         <v>0.089999999999999997</v>
@@ -2409,7 +2409,7 @@
         <v>23</v>
       </c>
       <c r="K48" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L48" s="0">
         <v>0.089999999999999997</v>
@@ -2456,7 +2456,7 @@
         <v>23</v>
       </c>
       <c r="K49" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L49" s="0">
         <v>0.10000000000000001</v>
@@ -2503,7 +2503,7 @@
         <v>23</v>
       </c>
       <c r="K50" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L50" s="0">
         <v>0.10000000000000001</v>
@@ -2550,7 +2550,7 @@
         <v>23</v>
       </c>
       <c r="K51" s="0">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="L51" s="0">
         <v>0.10000000000000001</v>

</xml_diff>

<commit_message>
add ITI jitter option
</commit_message>
<xml_diff>
--- a/rules/start-end effect/rules_SE.xlsx
+++ b/rules/start-end effect/rules_SE.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="32">
   <si>
     <t>pID</t>
   </si>
@@ -36,16 +36,25 @@
     <t>3-位置阶段(1k)</t>
   </si>
   <si>
-    <t>3-时长补充(1k)</t>
+    <t>4-时长补充(1k)</t>
   </si>
   <si>
-    <t>4-阈值阶段(4k)</t>
+    <t>5-阈值阶段(4k)</t>
+  </si>
+  <si>
+    <t>6-位置阶段EEG(1k)</t>
+  </si>
+  <si>
+    <t>7-时长补充EEG(1k)</t>
   </si>
   <si>
     <t>apType</t>
   </si>
   <si>
     <t>active</t>
+  </si>
+  <si>
+    <t>passive</t>
   </si>
   <si>
     <t>protocol</t>
@@ -64,6 +73,12 @@
   </si>
   <si>
     <t>SE th-4k</t>
+  </si>
+  <si>
+    <t>SE loc-EEG 1k</t>
+  </si>
+  <si>
+    <t>SE dur-EEG 1k</t>
   </si>
   <si>
     <t>code</t>
@@ -139,7 +154,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O113"/>
+  <dimension ref="A1:O137"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.15625" customWidth="true"/>
@@ -170,40 +185,40 @@
         <v>3</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -217,10 +232,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0">
         <v>4</v>
@@ -254,10 +269,10 @@
         <v>4</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0">
         <v>5</v>
@@ -297,10 +312,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F4" s="0">
         <v>6</v>
@@ -340,10 +355,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F5" s="0">
         <v>7</v>
@@ -383,10 +398,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F6" s="0">
         <v>8</v>
@@ -426,10 +441,10 @@
         <v>4</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F7" s="0">
         <v>9</v>
@@ -469,10 +484,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F8" s="0">
         <v>10</v>
@@ -512,10 +527,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F9" s="0">
         <v>11</v>
@@ -555,10 +570,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F10" s="0">
         <v>12</v>
@@ -598,10 +613,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F11" s="0">
         <v>13</v>
@@ -641,10 +656,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F12" s="0">
         <v>14</v>
@@ -684,10 +699,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F13" s="0">
         <v>15</v>
@@ -727,10 +742,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F14" s="0">
         <v>16</v>
@@ -770,10 +785,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F15" s="0">
         <v>17</v>
@@ -813,10 +828,10 @@
         <v>4</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F16" s="0">
         <v>18</v>
@@ -856,10 +871,10 @@
         <v>4</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F17" s="0">
         <v>19</v>
@@ -899,10 +914,10 @@
         <v>4</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F18" s="0">
         <v>20</v>
@@ -942,10 +957,10 @@
         <v>4</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F19" s="0">
         <v>21</v>
@@ -985,10 +1000,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F20" s="0">
         <v>22</v>
@@ -1028,10 +1043,10 @@
         <v>4</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F21" s="0">
         <v>23</v>
@@ -1071,10 +1086,10 @@
         <v>4</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F22" s="0">
         <v>24</v>
@@ -1114,10 +1129,10 @@
         <v>4</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F23" s="0">
         <v>25</v>
@@ -1157,10 +1172,10 @@
         <v>4</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F24" s="0">
         <v>26</v>
@@ -1200,10 +1215,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F25" s="0">
         <v>27</v>
@@ -1243,10 +1258,10 @@
         <v>4</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F26" s="0">
         <v>28</v>
@@ -1286,10 +1301,10 @@
         <v>4</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F27" s="0">
         <v>29</v>
@@ -1329,10 +1344,10 @@
         <v>4</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F28" s="0">
         <v>30</v>
@@ -1372,10 +1387,10 @@
         <v>4</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F29" s="0">
         <v>31</v>
@@ -1415,10 +1430,10 @@
         <v>4</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F30" s="0">
         <v>32</v>
@@ -1452,10 +1467,10 @@
         <v>4</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F31" s="0">
         <v>33</v>
@@ -1495,10 +1510,10 @@
         <v>4</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F32" s="0">
         <v>34</v>
@@ -1538,10 +1553,10 @@
         <v>4</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F33" s="0">
         <v>35</v>
@@ -1581,10 +1596,10 @@
         <v>4</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F34" s="0">
         <v>36</v>
@@ -1624,10 +1639,10 @@
         <v>4</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F35" s="0">
         <v>37</v>
@@ -1667,10 +1682,10 @@
         <v>4</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F36" s="0">
         <v>38</v>
@@ -1710,10 +1725,10 @@
         <v>4</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F37" s="0">
         <v>39</v>
@@ -1753,10 +1768,10 @@
         <v>4</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F38" s="0">
         <v>40</v>
@@ -1796,10 +1811,10 @@
         <v>4</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F39" s="0">
         <v>41</v>
@@ -1839,10 +1854,10 @@
         <v>4</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F40" s="0">
         <v>42</v>
@@ -1882,10 +1897,10 @@
         <v>4</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F41" s="0">
         <v>43</v>
@@ -1925,10 +1940,10 @@
         <v>4</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F42" s="0">
         <v>44</v>
@@ -1968,10 +1983,10 @@
         <v>4</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F43" s="0">
         <v>45</v>
@@ -2011,10 +2026,10 @@
         <v>4</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F44" s="0">
         <v>46</v>
@@ -2054,10 +2069,10 @@
         <v>4</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F45" s="0">
         <v>47</v>
@@ -2097,10 +2112,10 @@
         <v>4</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F46" s="0">
         <v>48</v>
@@ -2140,10 +2155,10 @@
         <v>4</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F47" s="0">
         <v>49</v>
@@ -2183,10 +2198,10 @@
         <v>4</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F48" s="0">
         <v>50</v>
@@ -2226,10 +2241,10 @@
         <v>4</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F49" s="0">
         <v>51</v>
@@ -2269,10 +2284,10 @@
         <v>4</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F50" s="0">
         <v>52</v>
@@ -2312,10 +2327,10 @@
         <v>4</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F51" s="0">
         <v>53</v>
@@ -2355,10 +2370,10 @@
         <v>4</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F52" s="0">
         <v>54</v>
@@ -2398,10 +2413,10 @@
         <v>4</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F53" s="0">
         <v>55</v>
@@ -2441,10 +2456,10 @@
         <v>4</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F54" s="0">
         <v>56</v>
@@ -2484,10 +2499,10 @@
         <v>4</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F55" s="0">
         <v>57</v>
@@ -2527,10 +2542,10 @@
         <v>4</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F56" s="0">
         <v>58</v>
@@ -2570,10 +2585,10 @@
         <v>4</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F57" s="0">
         <v>59</v>
@@ -2613,10 +2628,10 @@
         <v>5</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F58" s="0">
         <v>4</v>
@@ -2625,7 +2640,7 @@
         <v>3.5</v>
       </c>
       <c r="H58" s="0">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I58" s="0"/>
       <c r="J58" s="0"/>
@@ -2650,10 +2665,10 @@
         <v>5</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F59" s="0">
         <v>5</v>
@@ -2693,10 +2708,10 @@
         <v>5</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F60" s="0">
         <v>6</v>
@@ -2736,10 +2751,10 @@
         <v>5</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F61" s="0">
         <v>7</v>
@@ -2779,10 +2794,10 @@
         <v>5</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F62" s="0">
         <v>8</v>
@@ -2822,10 +2837,10 @@
         <v>5</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F63" s="0">
         <v>9</v>
@@ -2865,10 +2880,10 @@
         <v>5</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F64" s="0">
         <v>10</v>
@@ -2908,10 +2923,10 @@
         <v>5</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F65" s="0">
         <v>11</v>
@@ -2951,10 +2966,10 @@
         <v>5</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F66" s="0">
         <v>12</v>
@@ -2994,10 +3009,10 @@
         <v>5</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F67" s="0">
         <v>13</v>
@@ -3037,10 +3052,10 @@
         <v>5</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F68" s="0">
         <v>14</v>
@@ -3080,10 +3095,10 @@
         <v>5</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F69" s="0">
         <v>15</v>
@@ -3123,10 +3138,10 @@
         <v>5</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F70" s="0">
         <v>16</v>
@@ -3166,10 +3181,10 @@
         <v>5</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F71" s="0">
         <v>17</v>
@@ -3209,10 +3224,10 @@
         <v>5</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F72" s="0">
         <v>18</v>
@@ -3252,10 +3267,10 @@
         <v>5</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F73" s="0">
         <v>19</v>
@@ -3295,10 +3310,10 @@
         <v>6</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F74" s="0">
         <v>4</v>
@@ -3332,10 +3347,10 @@
         <v>6</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F75" s="0">
         <v>5</v>
@@ -3352,7 +3367,7 @@
         <v>1000</v>
       </c>
       <c r="L75" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M75" s="0">
         <v>20</v>
@@ -3375,10 +3390,10 @@
         <v>6</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F76" s="0">
         <v>6</v>
@@ -3395,7 +3410,7 @@
         <v>1000</v>
       </c>
       <c r="L76" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M76" s="0">
         <v>20</v>
@@ -3418,10 +3433,10 @@
         <v>6</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F77" s="0">
         <v>7</v>
@@ -3438,7 +3453,7 @@
         <v>1000</v>
       </c>
       <c r="L77" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M77" s="0">
         <v>20</v>
@@ -3461,10 +3476,10 @@
         <v>6</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F78" s="0">
         <v>8</v>
@@ -3481,7 +3496,7 @@
         <v>1000</v>
       </c>
       <c r="L78" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M78" s="0">
         <v>20</v>
@@ -3504,10 +3519,10 @@
         <v>6</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F79" s="0">
         <v>9</v>
@@ -3524,7 +3539,7 @@
         <v>1000</v>
       </c>
       <c r="L79" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M79" s="0">
         <v>20</v>
@@ -3547,10 +3562,10 @@
         <v>6</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F80" s="0">
         <v>10</v>
@@ -3567,7 +3582,7 @@
         <v>1000</v>
       </c>
       <c r="L80" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M80" s="0">
         <v>20</v>
@@ -3590,10 +3605,10 @@
         <v>6</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F81" s="0">
         <v>11</v>
@@ -3610,7 +3625,7 @@
         <v>1000</v>
       </c>
       <c r="L81" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M81" s="0">
         <v>20</v>
@@ -3633,10 +3648,10 @@
         <v>6</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F82" s="0">
         <v>12</v>
@@ -3653,7 +3668,7 @@
         <v>1000</v>
       </c>
       <c r="L82" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M82" s="0">
         <v>20</v>
@@ -3676,10 +3691,10 @@
         <v>6</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F83" s="0">
         <v>13</v>
@@ -3696,7 +3711,7 @@
         <v>1000</v>
       </c>
       <c r="L83" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M83" s="0">
         <v>20</v>
@@ -3719,10 +3734,10 @@
         <v>6</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F84" s="0">
         <v>14</v>
@@ -3739,7 +3754,7 @@
         <v>1000</v>
       </c>
       <c r="L84" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M84" s="0">
         <v>20</v>
@@ -3762,10 +3777,10 @@
         <v>6</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F85" s="0">
         <v>15</v>
@@ -3782,7 +3797,7 @@
         <v>1000</v>
       </c>
       <c r="L85" s="0">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="M85" s="0">
         <v>20</v>
@@ -3805,10 +3820,10 @@
         <v>7</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F86" s="0">
         <v>4</v>
@@ -3842,10 +3857,10 @@
         <v>7</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F87" s="0">
         <v>5</v>
@@ -3862,7 +3877,7 @@
         <v>1000</v>
       </c>
       <c r="L87" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M87" s="0">
         <v>20</v>
@@ -3885,10 +3900,10 @@
         <v>7</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F88" s="0">
         <v>6</v>
@@ -3905,7 +3920,7 @@
         <v>1000</v>
       </c>
       <c r="L88" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M88" s="0">
         <v>20</v>
@@ -3928,10 +3943,10 @@
         <v>7</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F89" s="0">
         <v>7</v>
@@ -3948,7 +3963,7 @@
         <v>1000</v>
       </c>
       <c r="L89" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M89" s="0">
         <v>20</v>
@@ -3971,10 +3986,10 @@
         <v>7</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F90" s="0">
         <v>8</v>
@@ -3991,7 +4006,7 @@
         <v>1000</v>
       </c>
       <c r="L90" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M90" s="0">
         <v>20</v>
@@ -4014,10 +4029,10 @@
         <v>7</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F91" s="0">
         <v>9</v>
@@ -4034,7 +4049,7 @@
         <v>1000</v>
       </c>
       <c r="L91" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M91" s="0">
         <v>20</v>
@@ -4057,10 +4072,10 @@
         <v>7</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F92" s="0">
         <v>10</v>
@@ -4077,7 +4092,7 @@
         <v>1000</v>
       </c>
       <c r="L92" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M92" s="0">
         <v>20</v>
@@ -4100,10 +4115,10 @@
         <v>7</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F93" s="0">
         <v>11</v>
@@ -4120,7 +4135,7 @@
         <v>1000</v>
       </c>
       <c r="L93" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M93" s="0">
         <v>20</v>
@@ -4143,10 +4158,10 @@
         <v>7</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F94" s="0">
         <v>12</v>
@@ -4163,7 +4178,7 @@
         <v>1000</v>
       </c>
       <c r="L94" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M94" s="0">
         <v>20</v>
@@ -4186,10 +4201,10 @@
         <v>7</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F95" s="0">
         <v>13</v>
@@ -4206,7 +4221,7 @@
         <v>1000</v>
       </c>
       <c r="L95" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M95" s="0">
         <v>20</v>
@@ -4229,10 +4244,10 @@
         <v>7</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F96" s="0">
         <v>14</v>
@@ -4249,7 +4264,7 @@
         <v>1000</v>
       </c>
       <c r="L96" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M96" s="0">
         <v>20</v>
@@ -4272,10 +4287,10 @@
         <v>7</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F97" s="0">
         <v>15</v>
@@ -4292,7 +4307,7 @@
         <v>1000</v>
       </c>
       <c r="L97" s="0">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="M97" s="0">
         <v>20</v>
@@ -4315,10 +4330,10 @@
         <v>8</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F98" s="0">
         <v>4</v>
@@ -4352,10 +4367,10 @@
         <v>8</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F99" s="0">
         <v>5</v>
@@ -4395,10 +4410,10 @@
         <v>8</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F100" s="0">
         <v>6</v>
@@ -4438,10 +4453,10 @@
         <v>8</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F101" s="0">
         <v>7</v>
@@ -4481,10 +4496,10 @@
         <v>8</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F102" s="0">
         <v>8</v>
@@ -4524,10 +4539,10 @@
         <v>8</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F103" s="0">
         <v>9</v>
@@ -4567,10 +4582,10 @@
         <v>8</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F104" s="0">
         <v>10</v>
@@ -4610,10 +4625,10 @@
         <v>8</v>
       </c>
       <c r="D105" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F105" s="0">
         <v>11</v>
@@ -4653,10 +4668,10 @@
         <v>8</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F106" s="0">
         <v>12</v>
@@ -4696,10 +4711,10 @@
         <v>8</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F107" s="0">
         <v>13</v>
@@ -4739,10 +4754,10 @@
         <v>8</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E108" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F108" s="0">
         <v>14</v>
@@ -4782,10 +4797,10 @@
         <v>8</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E109" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F109" s="0">
         <v>15</v>
@@ -4825,10 +4840,10 @@
         <v>8</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E110" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F110" s="0">
         <v>16</v>
@@ -4868,10 +4883,10 @@
         <v>8</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F111" s="0">
         <v>17</v>
@@ -4911,10 +4926,10 @@
         <v>8</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F112" s="0">
         <v>18</v>
@@ -4954,10 +4969,10 @@
         <v>8</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F113" s="0">
         <v>19</v>
@@ -4986,6 +5001,1026 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" s="0">
+        <v>165</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E114" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F114" s="0">
+        <v>4</v>
+      </c>
+      <c r="G114" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H114" s="0">
+        <v>40</v>
+      </c>
+      <c r="I114" s="0"/>
+      <c r="J114" s="0"/>
+      <c r="K114" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L114" s="0"/>
+      <c r="M114" s="0"/>
+      <c r="N114" s="0"/>
+      <c r="O114" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="0">
+        <v>165</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F115" s="0">
+        <v>5</v>
+      </c>
+      <c r="G115" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H115" s="0">
+        <v>40</v>
+      </c>
+      <c r="I115" s="0"/>
+      <c r="J115" s="0"/>
+      <c r="K115" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L115" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M115" s="0">
+        <v>20</v>
+      </c>
+      <c r="N115" s="0">
+        <v>5</v>
+      </c>
+      <c r="O115" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="0">
+        <v>165</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D116" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E116" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F116" s="0">
+        <v>6</v>
+      </c>
+      <c r="G116" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H116" s="0">
+        <v>40</v>
+      </c>
+      <c r="I116" s="0"/>
+      <c r="J116" s="0"/>
+      <c r="K116" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L116" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M116" s="0">
+        <v>20</v>
+      </c>
+      <c r="N116" s="0">
+        <v>10</v>
+      </c>
+      <c r="O116" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="0">
+        <v>165</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F117" s="0">
+        <v>7</v>
+      </c>
+      <c r="G117" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H117" s="0">
+        <v>40</v>
+      </c>
+      <c r="I117" s="0"/>
+      <c r="J117" s="0"/>
+      <c r="K117" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L117" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M117" s="0">
+        <v>20</v>
+      </c>
+      <c r="N117" s="0">
+        <v>15</v>
+      </c>
+      <c r="O117" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="0">
+        <v>165</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F118" s="0">
+        <v>8</v>
+      </c>
+      <c r="G118" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H118" s="0">
+        <v>40</v>
+      </c>
+      <c r="I118" s="0"/>
+      <c r="J118" s="0"/>
+      <c r="K118" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L118" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M118" s="0">
+        <v>20</v>
+      </c>
+      <c r="N118" s="0">
+        <v>20</v>
+      </c>
+      <c r="O118" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="0">
+        <v>165</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F119" s="0">
+        <v>9</v>
+      </c>
+      <c r="G119" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H119" s="0">
+        <v>40</v>
+      </c>
+      <c r="I119" s="0"/>
+      <c r="J119" s="0"/>
+      <c r="K119" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L119" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M119" s="0">
+        <v>20</v>
+      </c>
+      <c r="N119" s="0">
+        <v>30</v>
+      </c>
+      <c r="O119" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="0">
+        <v>165</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F120" s="0">
+        <v>10</v>
+      </c>
+      <c r="G120" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H120" s="0">
+        <v>40</v>
+      </c>
+      <c r="I120" s="0"/>
+      <c r="J120" s="0"/>
+      <c r="K120" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L120" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M120" s="0">
+        <v>20</v>
+      </c>
+      <c r="N120" s="0">
+        <v>50</v>
+      </c>
+      <c r="O120" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="0">
+        <v>165</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F121" s="0">
+        <v>11</v>
+      </c>
+      <c r="G121" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H121" s="0">
+        <v>40</v>
+      </c>
+      <c r="I121" s="0"/>
+      <c r="J121" s="0"/>
+      <c r="K121" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L121" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M121" s="0">
+        <v>20</v>
+      </c>
+      <c r="N121" s="0">
+        <v>70</v>
+      </c>
+      <c r="O121" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="0">
+        <v>165</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E122" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F122" s="0">
+        <v>12</v>
+      </c>
+      <c r="G122" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H122" s="0">
+        <v>40</v>
+      </c>
+      <c r="I122" s="0"/>
+      <c r="J122" s="0"/>
+      <c r="K122" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L122" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M122" s="0">
+        <v>20</v>
+      </c>
+      <c r="N122" s="0">
+        <v>80</v>
+      </c>
+      <c r="O122" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="0">
+        <v>165</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E123" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F123" s="0">
+        <v>13</v>
+      </c>
+      <c r="G123" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H123" s="0">
+        <v>40</v>
+      </c>
+      <c r="I123" s="0"/>
+      <c r="J123" s="0"/>
+      <c r="K123" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L123" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M123" s="0">
+        <v>20</v>
+      </c>
+      <c r="N123" s="0">
+        <v>85</v>
+      </c>
+      <c r="O123" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="0">
+        <v>165</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E124" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F124" s="0">
+        <v>14</v>
+      </c>
+      <c r="G124" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H124" s="0">
+        <v>40</v>
+      </c>
+      <c r="I124" s="0"/>
+      <c r="J124" s="0"/>
+      <c r="K124" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L124" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M124" s="0">
+        <v>20</v>
+      </c>
+      <c r="N124" s="0">
+        <v>90</v>
+      </c>
+      <c r="O124" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="0">
+        <v>165</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D125" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E125" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F125" s="0">
+        <v>15</v>
+      </c>
+      <c r="G125" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="H125" s="0">
+        <v>40</v>
+      </c>
+      <c r="I125" s="0"/>
+      <c r="J125" s="0"/>
+      <c r="K125" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L125" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M125" s="0">
+        <v>20</v>
+      </c>
+      <c r="N125" s="0">
+        <v>95</v>
+      </c>
+      <c r="O125" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="0">
+        <v>166</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D126" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E126" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F126" s="0">
+        <v>4</v>
+      </c>
+      <c r="G126" s="0">
+        <v>2</v>
+      </c>
+      <c r="H126" s="0">
+        <v>40</v>
+      </c>
+      <c r="I126" s="0"/>
+      <c r="J126" s="0"/>
+      <c r="K126" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L126" s="0"/>
+      <c r="M126" s="0"/>
+      <c r="N126" s="0"/>
+      <c r="O126" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="0">
+        <v>166</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D127" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E127" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F127" s="0">
+        <v>5</v>
+      </c>
+      <c r="G127" s="0">
+        <v>2</v>
+      </c>
+      <c r="H127" s="0">
+        <v>40</v>
+      </c>
+      <c r="I127" s="0"/>
+      <c r="J127" s="0"/>
+      <c r="K127" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L127" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M127" s="0">
+        <v>20</v>
+      </c>
+      <c r="N127" s="0">
+        <v>5</v>
+      </c>
+      <c r="O127" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="0">
+        <v>166</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D128" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E128" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F128" s="0">
+        <v>6</v>
+      </c>
+      <c r="G128" s="0">
+        <v>2</v>
+      </c>
+      <c r="H128" s="0">
+        <v>40</v>
+      </c>
+      <c r="I128" s="0"/>
+      <c r="J128" s="0"/>
+      <c r="K128" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L128" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M128" s="0">
+        <v>20</v>
+      </c>
+      <c r="N128" s="0">
+        <v>10</v>
+      </c>
+      <c r="O128" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="0">
+        <v>166</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D129" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E129" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F129" s="0">
+        <v>7</v>
+      </c>
+      <c r="G129" s="0">
+        <v>2</v>
+      </c>
+      <c r="H129" s="0">
+        <v>40</v>
+      </c>
+      <c r="I129" s="0"/>
+      <c r="J129" s="0"/>
+      <c r="K129" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L129" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M129" s="0">
+        <v>20</v>
+      </c>
+      <c r="N129" s="0">
+        <v>15</v>
+      </c>
+      <c r="O129" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="0">
+        <v>166</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D130" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E130" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F130" s="0">
+        <v>8</v>
+      </c>
+      <c r="G130" s="0">
+        <v>2</v>
+      </c>
+      <c r="H130" s="0">
+        <v>40</v>
+      </c>
+      <c r="I130" s="0"/>
+      <c r="J130" s="0"/>
+      <c r="K130" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L130" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M130" s="0">
+        <v>20</v>
+      </c>
+      <c r="N130" s="0">
+        <v>20</v>
+      </c>
+      <c r="O130" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="0">
+        <v>166</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D131" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E131" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F131" s="0">
+        <v>9</v>
+      </c>
+      <c r="G131" s="0">
+        <v>2</v>
+      </c>
+      <c r="H131" s="0">
+        <v>40</v>
+      </c>
+      <c r="I131" s="0"/>
+      <c r="J131" s="0"/>
+      <c r="K131" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L131" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M131" s="0">
+        <v>20</v>
+      </c>
+      <c r="N131" s="0">
+        <v>30</v>
+      </c>
+      <c r="O131" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="0">
+        <v>166</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D132" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E132" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F132" s="0">
+        <v>10</v>
+      </c>
+      <c r="G132" s="0">
+        <v>2</v>
+      </c>
+      <c r="H132" s="0">
+        <v>40</v>
+      </c>
+      <c r="I132" s="0"/>
+      <c r="J132" s="0"/>
+      <c r="K132" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L132" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M132" s="0">
+        <v>20</v>
+      </c>
+      <c r="N132" s="0">
+        <v>50</v>
+      </c>
+      <c r="O132" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="0">
+        <v>166</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E133" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F133" s="0">
+        <v>11</v>
+      </c>
+      <c r="G133" s="0">
+        <v>2</v>
+      </c>
+      <c r="H133" s="0">
+        <v>40</v>
+      </c>
+      <c r="I133" s="0"/>
+      <c r="J133" s="0"/>
+      <c r="K133" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L133" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M133" s="0">
+        <v>20</v>
+      </c>
+      <c r="N133" s="0">
+        <v>70</v>
+      </c>
+      <c r="O133" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="0">
+        <v>166</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C134" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D134" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E134" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F134" s="0">
+        <v>12</v>
+      </c>
+      <c r="G134" s="0">
+        <v>2</v>
+      </c>
+      <c r="H134" s="0">
+        <v>40</v>
+      </c>
+      <c r="I134" s="0"/>
+      <c r="J134" s="0"/>
+      <c r="K134" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L134" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M134" s="0">
+        <v>20</v>
+      </c>
+      <c r="N134" s="0">
+        <v>80</v>
+      </c>
+      <c r="O134" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="0">
+        <v>166</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D135" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E135" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F135" s="0">
+        <v>13</v>
+      </c>
+      <c r="G135" s="0">
+        <v>2</v>
+      </c>
+      <c r="H135" s="0">
+        <v>40</v>
+      </c>
+      <c r="I135" s="0"/>
+      <c r="J135" s="0"/>
+      <c r="K135" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L135" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M135" s="0">
+        <v>20</v>
+      </c>
+      <c r="N135" s="0">
+        <v>85</v>
+      </c>
+      <c r="O135" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="0">
+        <v>166</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D136" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E136" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F136" s="0">
+        <v>14</v>
+      </c>
+      <c r="G136" s="0">
+        <v>2</v>
+      </c>
+      <c r="H136" s="0">
+        <v>40</v>
+      </c>
+      <c r="I136" s="0"/>
+      <c r="J136" s="0"/>
+      <c r="K136" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L136" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M136" s="0">
+        <v>20</v>
+      </c>
+      <c r="N136" s="0">
+        <v>90</v>
+      </c>
+      <c r="O136" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="0">
+        <v>166</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D137" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E137" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F137" s="0">
+        <v>15</v>
+      </c>
+      <c r="G137" s="0">
+        <v>2</v>
+      </c>
+      <c r="H137" s="0">
+        <v>40</v>
+      </c>
+      <c r="I137" s="0"/>
+      <c r="J137" s="0"/>
+      <c r="K137" s="0">
+        <v>1000</v>
+      </c>
+      <c r="L137" s="0">
+        <v>1020</v>
+      </c>
+      <c r="M137" s="0">
+        <v>20</v>
+      </c>
+      <c r="N137" s="0">
+        <v>95</v>
+      </c>
+      <c r="O137" s="0">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update for 2 channel wave
</commit_message>
<xml_diff>
--- a/rules/start-end effect/rules_SE.xlsx
+++ b/rules/start-end effect/rules_SE.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="559" uniqueCount="32">
   <si>
     <t>pID</t>
   </si>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -153,25 +153,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O137"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.15625" customWidth="true"/>
-    <col min="2" max="2" width="12.6015625" customWidth="true"/>
-    <col min="3" max="3" width="17.046875" customWidth="true"/>
-    <col min="4" max="4" width="7.046875" customWidth="true"/>
-    <col min="5" max="5" width="14.7109375" customWidth="true"/>
-    <col min="6" max="6" width="5.15625" customWidth="true"/>
-    <col min="7" max="7" width="3.7109375" customWidth="true"/>
-    <col min="8" max="8" width="7.93359375" customWidth="true"/>
-    <col min="9" max="9" width="6.82421875" customWidth="true"/>
-    <col min="10" max="10" width="10.15625" customWidth="true"/>
-    <col min="11" max="11" width="5.15625" customWidth="true"/>
-    <col min="12" max="12" width="5.15625" customWidth="true"/>
-    <col min="13" max="13" width="13.37890625" customWidth="true"/>
-    <col min="14" max="14" width="4.046875" customWidth="true"/>
-    <col min="15" max="15" width="3.82421875" customWidth="true"/>
+    <col min="1" max="1" width="4" customWidth="true"/>
+    <col min="2" max="2" width="12.44140625" customWidth="true"/>
+    <col min="3" max="3" width="16.88671875" customWidth="true"/>
+    <col min="4" max="4" width="6.88671875" customWidth="true"/>
+    <col min="5" max="5" width="14.5546875" customWidth="true"/>
+    <col min="6" max="6" width="5" customWidth="true"/>
+    <col min="7" max="7" width="3.5546875" customWidth="true"/>
+    <col min="8" max="8" width="7.77734375" customWidth="true"/>
+    <col min="9" max="9" width="6.6640625" customWidth="true"/>
+    <col min="10" max="10" width="10" customWidth="true"/>
+    <col min="11" max="11" width="5" customWidth="true"/>
+    <col min="12" max="12" width="5" customWidth="true"/>
+    <col min="13" max="13" width="13.21875" customWidth="true"/>
+    <col min="14" max="14" width="3.88671875" customWidth="true"/>
+    <col min="15" max="15" width="3.6640625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5579,7 +5582,7 @@
         <v>1000</v>
       </c>
       <c r="L127" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M127" s="0">
         <v>20</v>
@@ -5622,7 +5625,7 @@
         <v>1000</v>
       </c>
       <c r="L128" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M128" s="0">
         <v>20</v>
@@ -5665,7 +5668,7 @@
         <v>1000</v>
       </c>
       <c r="L129" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M129" s="0">
         <v>20</v>
@@ -5708,7 +5711,7 @@
         <v>1000</v>
       </c>
       <c r="L130" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M130" s="0">
         <v>20</v>
@@ -5751,7 +5754,7 @@
         <v>1000</v>
       </c>
       <c r="L131" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M131" s="0">
         <v>20</v>
@@ -5794,7 +5797,7 @@
         <v>1000</v>
       </c>
       <c r="L132" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M132" s="0">
         <v>20</v>
@@ -5837,7 +5840,7 @@
         <v>1000</v>
       </c>
       <c r="L133" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M133" s="0">
         <v>20</v>
@@ -5880,7 +5883,7 @@
         <v>1000</v>
       </c>
       <c r="L134" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M134" s="0">
         <v>20</v>
@@ -5923,7 +5926,7 @@
         <v>1000</v>
       </c>
       <c r="L135" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M135" s="0">
         <v>20</v>
@@ -5966,7 +5969,7 @@
         <v>1000</v>
       </c>
       <c r="L136" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M136" s="0">
         <v>20</v>
@@ -6009,7 +6012,7 @@
         <v>1000</v>
       </c>
       <c r="L137" s="0">
-        <v>1020</v>
+        <v>1060</v>
       </c>
       <c r="M137" s="0">
         <v>20</v>

</xml_diff>